<commit_message>
Added 2 more test cases related to sign-in & sign out
</commit_message>
<xml_diff>
--- a/Assignment_1.xlsx
+++ b/Assignment_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jinesh/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jinesh/Data/Study/Automation/loginext-tasks-by-jinesh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8F922D-4C74-3E4A-99E6-73CEED9D851C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB02136-E415-D045-88B4-D7EA484F3C3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16080" activeTab="1" xr2:uid="{0844A80C-7F68-E046-B4C9-C18CD77EF643}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16080" xr2:uid="{0844A80C-7F68-E046-B4C9-C18CD77EF643}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="286">
   <si>
     <t>Sr No</t>
   </si>
@@ -931,6 +931,50 @@
   </si>
   <si>
     <t>NOTE: For preconditions, test steps, test data &amp; expected results of non-functional testing, I would need more time &amp; discussion with the team</t>
+  </si>
+  <si>
+    <t>TCF0038</t>
+  </si>
+  <si>
+    <t>1. App has been successfully installed on the phone</t>
+  </si>
+  <si>
+    <t>Verify that the agent/manager is able to sign-in or sign-up in the app with correct credentials</t>
+  </si>
+  <si>
+    <t>1. Install the app on the phone
+2. Open the app
+3. Sign-in or Sign-up with correct credentials</t>
+  </si>
+  <si>
+    <t>Valid email/username &amp; password
+Invalid email/username &amp; password
+Valid email/username &amp; invalid password</t>
+  </si>
+  <si>
+    <t>User is able to successfully sign-in or sign-up in the app</t>
+  </si>
+  <si>
+    <t>TCF0039</t>
+  </si>
+  <si>
+    <t>Sign out/Logout option</t>
+  </si>
+  <si>
+    <t>1. App has been successfully installed on the phone
+2. Agent/manager has signed-in to the app</t>
+  </si>
+  <si>
+    <t>Verify that there is an option to logout/sign out from the app</t>
+  </si>
+  <si>
+    <t>1. Install the app on the phone
+2. Open the app
+3. Sign-in or Sign-up with correct credentials
+4. Option to Logout/Sign out</t>
+  </si>
+  <si>
+    <t>User is redirected to the login pafge once he/she logs out from the app</t>
   </si>
 </sst>
 </file>
@@ -981,7 +1025,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1004,11 +1048,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1029,6 +1086,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1343,10 +1412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97485E1-0617-BA45-87F1-E75A8B7CD690}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1414,7 +1483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f>A2+1</f>
         <v>2</v>
@@ -1426,130 +1495,130 @@
         <v>31</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>63</v>
+        <v>276</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>138</v>
+        <v>277</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="200" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A38" si="0">A3+1</f>
+        <f t="shared" ref="A4:A5" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>62</v>
+        <v>283</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>139</v>
+        <v>284</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="100" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>269</v>
+        <v>63</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>270</v>
+        <v>138</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="200" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A6:A40" si="1">A5+1</f>
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>263</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>140</v>
+        <v>266</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="G6" s="4"/>
+        <v>139</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>265</v>
+      </c>
       <c r="H6" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="100" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>267</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>142</v>
+        <v>268</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>7</v>
+        <v>269</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>141</v>
+        <v>270</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>143</v>
+        <v>271</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="80" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1559,24 +1628,22 @@
         <v>36</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>147</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="80" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1586,22 +1653,24 @@
         <v>37</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="G9" s="5"/>
+        <v>141</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="H9" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="160" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="80" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1611,24 +1680,24 @@
         <v>38</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="140" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="80" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1638,24 +1707,22 @@
         <v>39</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>121</v>
+        <v>11</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>158</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="G11" s="5"/>
       <c r="H11" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="80" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="160" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1665,24 +1732,24 @@
         <v>40</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="140" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1692,24 +1759,24 @@
         <v>41</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>204</v>
+        <v>153</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>165</v>
+        <v>121</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="100" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="80" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1719,78 +1786,78 @@
         <v>42</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>166</v>
+        <v>13</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>123</v>
+        <v>9</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>172</v>
+        <v>204</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="100" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="40" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
       <c r="B16" s="4" t="s">
-        <v>123</v>
+        <v>9</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>22</v>
+        <v>166</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="160" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1800,53 +1867,55 @@
         <v>45</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="100" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="40" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G18" s="4"/>
+        <v>176</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>177</v>
+      </c>
       <c r="H18" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="280" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="160" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>47</v>
@@ -1855,75 +1924,73 @@
         <v>153</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="100" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>214</v>
+        <v>153</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>222</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="G20" s="4"/>
       <c r="H20" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="100" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="280" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>215</v>
+        <v>153</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>222</v>
+        <v>185</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="160" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1933,24 +2000,24 @@
         <v>50</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>222</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="100" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -1960,24 +2027,24 @@
         <v>51</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="160" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1987,24 +2054,24 @@
         <v>52</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="100" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -2014,24 +2081,24 @@
         <v>53</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>126</v>
+        <v>20</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -2041,76 +2108,78 @@
         <v>54</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>187</v>
+        <v>20</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="100" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>219</v>
+        <v>126</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="G27" s="4"/>
+        <v>205</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>223</v>
+      </c>
       <c r="H27" s="4" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>127</v>
+        <v>187</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="100" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -2120,49 +2189,49 @@
         <v>119</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>128</v>
+        <v>219</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>227</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="G29" s="4"/>
       <c r="H29" s="4" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="C30" s="4" t="s">
         <v>120</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>238</v>
+        <v>127</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="100" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -2175,21 +2244,21 @@
         <v>231</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>233</v>
+        <v>128</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B32" s="4"/>
@@ -2197,28 +2266,28 @@
         <v>125</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="100" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>196</v>
@@ -2227,48 +2296,46 @@
         <v>231</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>129</v>
+        <v>233</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
         <v>197</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>130</v>
+        <v>239</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="80" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -2281,21 +2348,21 @@
         <v>231</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="100" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -2308,21 +2375,21 @@
         <v>231</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>240</v>
+        <v>130</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="80" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -2332,24 +2399,24 @@
         <v>200</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>236</v>
+        <v>23</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="100" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -2359,44 +2426,78 @@
         <v>201</v>
       </c>
       <c r="D38" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E40" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F40" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="G40" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="H38" s="4" t="s">
+      <c r="H40" s="4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-    </row>
-    <row r="40" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-    </row>
     <row r="41" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -2404,119 +2505,119 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="20" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>255</v>
-      </c>
+    <row r="42" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="20" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>261</v>
-      </c>
+    <row r="43" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" ht="20" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>261</v>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>255</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:8" ht="20" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="4" t="s">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="11" t="s">
         <v>257</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8" ht="20" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="4" t="s">
-        <v>259</v>
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="11" t="s">
+        <v>257</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>262</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
+    <row r="47" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>262</v>
+      </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
+    <row r="48" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>262</v>
+      </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -2525,8 +2626,8 @@
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -2535,8 +2636,8 @@
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -2545,14 +2646,58 @@
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A55" s="12"/>
+      <c r="B55" s="13"/>
+    </row>
+    <row r="56" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A56" s="12"/>
+      <c r="B56" s="13"/>
+    </row>
+    <row r="57" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A57" s="12"/>
+      <c r="B57" s="13"/>
+    </row>
+    <row r="58" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A58" s="12"/>
+      <c r="B58" s="13"/>
+    </row>
+    <row r="59" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A59" s="12"/>
+      <c r="B59" s="13"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="13"/>
+      <c r="B60" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2564,7 +2709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D167DB65-C94B-F94B-9AC5-35C6BAA761DC}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>

</xml_diff>